<commit_message>
empaquetamiento de plantaillas y Event Storming
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominioEnriquecido/ModeloDominioEnriquecido-Inventario.xlsx
+++ b/SpaOnline/ModeloDominioEnriquecido/ModeloDominioEnriquecido-Inventario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/ModeloDominioEnriquecido/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{9676E325-C85E-4257-A0EF-CEADE506081E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{455837DE-F4EF-4AB3-A378-8A74E820811D}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{9676E325-C85E-4257-A0EF-CEADE506081E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D37B911D-FFD5-45FA-B0AF-FFE783E6CF46}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4815" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de dominio anémico" sheetId="61" r:id="rId1"/>
@@ -251,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,12 +305,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -702,6 +696,63 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -723,65 +774,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1173,7 +1167,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,9 +1189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02388B9D-0652-49D5-BF62-A59B793D6DFC}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,13 +1220,13 @@
       <c r="A2" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="53" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1243,10 +1237,10 @@
       <c r="B3" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="53" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1265,7 +1259,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C13" sqref="C13:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,69 +1289,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="55" t="str">
+      <c r="B3" s="74" t="str">
         <f>'Listado Objetos de Dominio'!$B$2</f>
         <v>Objeto de dominio que contiene la informacion del inventario, según el producto y sucursal</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1512,11 +1506,11 @@
       <c r="T6" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="77"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
@@ -1541,44 +1535,44 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60" t="s">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60" t="s">
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60" t="s">
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60" t="s">
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60" t="s">
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="R13" s="63"/>
+      <c r="R13" s="67"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
       <c r="G14" s="19" t="s">
         <v>28</v>
       </c>
@@ -1591,12 +1585,12 @@
       <c r="J14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="62" t="s">
+      <c r="K14" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
       <c r="O14" s="19" t="s">
         <v>30</v>
       </c>
@@ -1611,88 +1605,88 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
+      <c r="A15" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="65"/>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
       <c r="G15" s="20"/>
       <c r="H15" s="21"/>
       <c r="I15" s="22"/>
       <c r="J15" s="21"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="66"/>
-      <c r="N15" s="66"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="26"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="77"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
       <c r="G16" s="46"/>
       <c r="H16" s="44"/>
       <c r="I16" s="45"/>
       <c r="J16" s="39"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="71"/>
-      <c r="N16" s="71"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
       <c r="O16" s="23"/>
       <c r="P16" s="24"/>
       <c r="Q16" s="24"/>
       <c r="R16" s="27"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="73"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
       <c r="G17" s="42"/>
       <c r="H17" s="40"/>
       <c r="I17" s="41"/>
       <c r="J17" s="43"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
       <c r="O17" s="28"/>
       <c r="P17" s="29"/>
       <c r="Q17" s="29"/>
       <c r="R17" s="30"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="48"/>
       <c r="H18" s="49"/>
       <c r="I18" s="47"/>
       <c r="J18" s="48"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
       <c r="O18" s="31"/>
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
@@ -1700,6 +1694,20 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A13:B14"/>
+    <mergeCell ref="C13:F14"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="K15:N15"/>
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:F18"/>
@@ -1709,20 +1717,6 @@
     <mergeCell ref="K17:N17"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:F16"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A13:B14"/>
-    <mergeCell ref="C13:F14"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="O13:P13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{F92E8141-0BAA-4CFF-A2AA-790349ADA214}"/>
@@ -1746,7 +1740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
@@ -1778,70 +1772,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="54" t="str">
+      <c r="B2" s="73" t="str">
         <f>'Listado Objetos de Dominio'!$A$3</f>
         <v>ProductoInventario</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="55" t="str">
+      <c r="B3" s="74" t="str">
         <f>'Listado Objetos de Dominio'!$B$3</f>
         <v xml:space="preserve">Objeto de dominio que referencia los productos que tiene el inventario </v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2025,11 +2019,11 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="77"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
@@ -2048,44 +2042,44 @@
       <c r="C12" s="38"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60" t="s">
+      <c r="B14" s="66"/>
+      <c r="C14" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60" t="s">
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60" t="s">
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60" t="s">
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60" t="s">
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="63"/>
+      <c r="R14" s="67"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
       <c r="G15" s="19" t="s">
         <v>28</v>
       </c>
@@ -2098,12 +2092,12 @@
       <c r="J15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="62" t="s">
+      <c r="K15" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
       <c r="O15" s="19" t="s">
         <v>30</v>
       </c>
@@ -2118,88 +2112,88 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="26"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="46"/>
       <c r="H17" s="44"/>
       <c r="I17" s="45"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="27"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
       <c r="G18" s="42"/>
       <c r="H18" s="40"/>
       <c r="I18" s="41"/>
       <c r="J18" s="43"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="62"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
       <c r="O19" s="31"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>
@@ -2207,6 +2201,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="K16:N16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="K17:N17"/>
@@ -2219,17 +2224,6 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="J14:N14"/>
     <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K19:N19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{BD3FFCC5-4B44-4838-A36D-76DB08190487}"/>
@@ -2249,12 +2243,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2402,15 +2393,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2434,10 +2429,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>